<commit_message>
design finished, simulation started
</commit_message>
<xml_diff>
--- a/documents/Rhodotron Parametreler (v5).xlsx
+++ b/documents/Rhodotron Parametreler (v5).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cernbox\cernbox\Rhodotron\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Repos\MSThesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B803451D-FDC2-48F3-91EF-4A987D810D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AE587A-32BB-4D47-8742-3DA4E9AA6100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A977ED4B-B779-4DB6-A8B8-B7CE20AE608B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A977ED4B-B779-4DB6-A8B8-B7CE20AE608B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
   <si>
     <t>T (ns)</t>
   </si>
@@ -2236,7 +2236,7 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2296,9 +2296,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="9" xfId="7" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
@@ -2332,13 +2331,30 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2357,18 +2373,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2383,12 +2387,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2522,8 +2520,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16501677" y="2314576"/>
-          <a:ext cx="3303948" cy="2867984"/>
+          <a:off x="16593565" y="2590801"/>
+          <a:ext cx="3242316" cy="2862941"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2535,15 +2533,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>433667</xdr:colOff>
+      <xdr:colOff>419380</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>6483</xdr:rowOff>
+      <xdr:rowOff>16008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>293914</xdr:colOff>
+      <xdr:colOff>279627</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>3329</xdr:rowOff>
+      <xdr:rowOff>12854</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2571,8 +2569,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13309226" y="2572630"/>
-          <a:ext cx="3199600" cy="2887964"/>
+          <a:off x="13401955" y="2578233"/>
+          <a:ext cx="3184472" cy="2882921"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2881,10 +2879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65439ADF-7CD5-4C3B-BCA2-78038D935A1F}">
-  <dimension ref="A1:Y36"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2909,33 +2907,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="48"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="52"/>
     </row>
     <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
@@ -2949,26 +2947,26 @@
         <v>5</v>
       </c>
       <c r="G2" s="17"/>
-      <c r="H2" s="63" t="s">
+      <c r="H2" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="22"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="21"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
@@ -2981,12 +2979,12 @@
       <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="22"/>
       <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="17"/>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="41" t="s">
         <v>41</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -2998,10 +2996,10 @@
       <c r="K3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="66" t="s">
+      <c r="L3" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="67"/>
+      <c r="M3" s="65"/>
       <c r="N3" s="2" t="s">
         <v>46</v>
       </c>
@@ -3017,13 +3015,8 @@
       <c r="R3" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="22"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="21"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
@@ -3038,7 +3031,7 @@
         <f>(E24/1000000)/B4</f>
         <v>2.7887670511627909</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
@@ -3052,52 +3045,47 @@
       </c>
       <c r="J4" s="11">
         <f>P4/0.5109989461</f>
-        <v>2.1926000833501558</v>
+        <v>2.1046988689744164</v>
       </c>
       <c r="K4" s="11">
         <f>SQRT(1-(1/(J4*J4)))</f>
-        <v>0.88993902530456559</v>
-      </c>
-      <c r="L4" s="54">
+        <v>0.87991704128853487</v>
+      </c>
+      <c r="L4" s="48">
         <f>B18</f>
         <v>0.04</v>
       </c>
-      <c r="M4" s="55"/>
+      <c r="M4" s="49"/>
       <c r="N4" s="11">
         <f>C18</f>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O4" s="11">
         <f t="shared" ref="O4:O13" si="0">L4+N4</f>
-        <v>0.6094173857107017</v>
+        <v>0.56449995780378892</v>
       </c>
       <c r="P4" s="12">
         <f t="shared" ref="P4:P13" si="1">O4+0.5109989461</f>
-        <v>1.1204163318107017</v>
+        <v>1.0754989039037888</v>
       </c>
       <c r="Q4" s="12">
         <f>9.10938356*10^(-31)*J4*299792458*K4/(1.60217662*10^(-19)*D15)</f>
-        <v>1.3273159680222649E-2</v>
+        <v>1.2597557158046826E-2</v>
       </c>
       <c r="R4" s="12">
         <f>Q4*10000</f>
-        <v>132.73159680222648</v>
-      </c>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="22"/>
+        <v>125.97557158046826</v>
+      </c>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="21"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="39"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="38"/>
       <c r="G5" s="17"/>
       <c r="H5" s="11">
         <v>2</v>
@@ -3108,44 +3096,39 @@
       </c>
       <c r="J5" s="11">
         <f t="shared" ref="J5:J13" si="3">P5/0.5109989461</f>
-        <v>3.3069221187605176</v>
+        <v>3.1311196900090397</v>
       </c>
       <c r="K5" s="11">
         <f t="shared" ref="K5:K13" si="4">SQRT(1-(1/(J5*J5)))</f>
-        <v>0.95318238707455061</v>
-      </c>
-      <c r="L5" s="54">
+        <v>0.94762855854960959</v>
+      </c>
+      <c r="L5" s="48">
         <f t="shared" ref="L5:L13" si="5">O4</f>
-        <v>0.6094173857107017</v>
-      </c>
-      <c r="M5" s="55"/>
+        <v>0.56449995780378892</v>
+      </c>
+      <c r="M5" s="49"/>
       <c r="N5" s="11">
         <f>N4</f>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O5" s="11">
         <f t="shared" si="0"/>
-        <v>1.1788347714214034</v>
+        <v>1.0889999156075778</v>
       </c>
       <c r="P5" s="11">
         <f t="shared" si="1"/>
-        <v>1.6898337175214033</v>
+        <v>1.5999988617075778</v>
       </c>
       <c r="Q5" s="11">
         <f>9.10938356*10^(-31)*J5*299792458*K5/(1.60217662*10^(-19)*D15)</f>
-        <v>2.1441472973035891E-2</v>
+        <v>2.0183312797937007E-2</v>
       </c>
       <c r="R5" s="11">
         <f t="shared" ref="R5:R13" si="6">Q5*10000</f>
-        <v>214.41472973035891</v>
-      </c>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="22"/>
+        <v>201.83312797937006</v>
+      </c>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="21"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
@@ -3158,8 +3141,8 @@
       <c r="D6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="40"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="11">
         <v>3</v>
@@ -3170,61 +3153,55 @@
       </c>
       <c r="J6" s="11">
         <f t="shared" si="3"/>
-        <v>4.4212441541708793</v>
+        <v>4.1575405110436625</v>
       </c>
       <c r="K6" s="11">
         <f t="shared" si="4"/>
-        <v>0.97408536635130849</v>
-      </c>
-      <c r="L6" s="54">
+        <v>0.97064249270561198</v>
+      </c>
+      <c r="L6" s="48">
         <f t="shared" si="5"/>
-        <v>1.1788347714214034</v>
-      </c>
-      <c r="M6" s="55"/>
+        <v>1.0889999156075778</v>
+      </c>
+      <c r="M6" s="49"/>
       <c r="N6" s="11">
         <f t="shared" ref="N6:N13" si="7">N5</f>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O6" s="11">
         <f t="shared" si="0"/>
-        <v>1.748252157132105</v>
+        <v>1.6134998734113668</v>
       </c>
       <c r="P6" s="11">
         <f t="shared" si="1"/>
-        <v>2.259251103232105</v>
+        <v>2.1244988195113668</v>
       </c>
       <c r="Q6" s="11">
         <f>9.10938356*10^(-31)*J6*299792458*K6/(1.60217662*10^(-19)*D15)</f>
-        <v>2.9295179184080387E-2</v>
+        <v>2.7450510829572693E-2</v>
       </c>
       <c r="R6" s="11">
         <f t="shared" si="6"/>
-        <v>292.95179184080388</v>
-      </c>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="22"/>
+        <v>274.50510829572693</v>
+      </c>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="21"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="1">
         <f>C7+D7</f>
-        <v>63.169025885585256</v>
+        <v>39.186999746822735</v>
       </c>
       <c r="C7" s="1">
-        <f>42.43</f>
-        <v>42.43</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1">
         <f>E18*E21</f>
-        <v>20.73902588558526</v>
-      </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="40"/>
+        <v>3.1869997468227336</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="11">
         <v>4</v>
@@ -3235,52 +3212,47 @@
       </c>
       <c r="J7" s="11">
         <f t="shared" si="3"/>
-        <v>5.5355661895812407</v>
+        <v>5.1839613320782849</v>
       </c>
       <c r="K7" s="11">
         <f t="shared" si="4"/>
-        <v>0.98354744654147364</v>
-      </c>
-      <c r="L7" s="54">
+        <v>0.98121789556513939</v>
+      </c>
+      <c r="L7" s="48">
         <f t="shared" si="5"/>
-        <v>1.748252157132105</v>
-      </c>
-      <c r="M7" s="55"/>
+        <v>1.6134998734113668</v>
+      </c>
+      <c r="M7" s="49"/>
       <c r="N7" s="11">
         <f t="shared" si="7"/>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O7" s="11">
         <f t="shared" si="0"/>
-        <v>2.3176695428428067</v>
+        <v>2.1379998312151556</v>
       </c>
       <c r="P7" s="11">
         <f t="shared" si="1"/>
-        <v>2.8286684889428066</v>
+        <v>2.6489987773151555</v>
       </c>
       <c r="Q7" s="11">
         <f>9.10938356*10^(-31)*J7*299792458*K7/(1.60217662*10^(-19)*D15)</f>
-        <v>3.7034970614522322E-2</v>
+        <v>3.4600458584614406E-2</v>
       </c>
       <c r="R7" s="11">
         <f t="shared" si="6"/>
-        <v>370.34970614522319</v>
-      </c>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="22"/>
+        <v>346.00458584614404</v>
+      </c>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="21"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="39"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="17"/>
       <c r="H8" s="11">
         <v>5</v>
@@ -3291,44 +3263,39 @@
       </c>
       <c r="J8" s="11">
         <f t="shared" si="3"/>
-        <v>6.6498882249916029</v>
+        <v>6.2103821531129073</v>
       </c>
       <c r="K8" s="11">
         <f t="shared" si="4"/>
-        <v>0.98862850278901437</v>
-      </c>
-      <c r="L8" s="54">
+        <v>0.98695103140982687</v>
+      </c>
+      <c r="L8" s="48">
         <f t="shared" si="5"/>
-        <v>2.3176695428428067</v>
-      </c>
-      <c r="M8" s="55"/>
+        <v>2.1379998312151556</v>
+      </c>
+      <c r="M8" s="49"/>
       <c r="N8" s="11">
         <f t="shared" si="7"/>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O8" s="11">
         <f t="shared" si="0"/>
-        <v>2.8870869285535083</v>
+        <v>2.6624997890189444</v>
       </c>
       <c r="P8" s="11">
         <f t="shared" si="1"/>
-        <v>3.3980858746535083</v>
+        <v>3.1734987351189443</v>
       </c>
       <c r="Q8" s="11">
         <f>9.10938356*10^(-31)*J8*299792458*K8/(1.60217662*10^(-19)*D15)</f>
-        <v>4.4720032851361988E-2</v>
+        <v>4.1693520886137168E-2</v>
       </c>
       <c r="R8" s="11">
         <f t="shared" si="6"/>
-        <v>447.20032851361987</v>
-      </c>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="32"/>
-      <c r="Y8" s="22"/>
+        <v>416.93520886137168</v>
+      </c>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="21"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
@@ -3344,7 +3311,7 @@
       <c r="E9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="11">
         <v>6</v>
@@ -3355,44 +3322,39 @@
       </c>
       <c r="J9" s="11">
         <f t="shared" si="3"/>
-        <v>7.7642102604019643</v>
+        <v>7.2368029741475297</v>
       </c>
       <c r="K9" s="11">
         <f t="shared" si="4"/>
-        <v>0.99167109701853262</v>
-      </c>
-      <c r="L9" s="54">
+        <v>0.99040677432531854</v>
+      </c>
+      <c r="L9" s="48">
         <f t="shared" si="5"/>
-        <v>2.8870869285535083</v>
-      </c>
-      <c r="M9" s="55"/>
+        <v>2.6624997890189444</v>
+      </c>
+      <c r="M9" s="49"/>
       <c r="N9" s="11">
         <f t="shared" si="7"/>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O9" s="11">
         <f t="shared" si="0"/>
-        <v>3.45650431426421</v>
+        <v>3.1869997468227331</v>
       </c>
       <c r="P9" s="11">
         <f t="shared" si="1"/>
-        <v>3.96750326036421</v>
+        <v>3.6979986929227331</v>
       </c>
       <c r="Q9" s="11">
         <f>9.10938356*10^(-31)*J9*299792458*K9/(1.60217662*10^(-19)*D15)</f>
-        <v>5.2374463174838043E-2</v>
+        <v>4.8754532031965031E-2</v>
       </c>
       <c r="R9" s="11">
         <f t="shared" si="6"/>
-        <v>523.74463174838047</v>
-      </c>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="32"/>
-      <c r="Y9" s="22"/>
+        <v>487.54532031965033</v>
+      </c>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="21"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
@@ -3412,7 +3374,7 @@
         <f>PI()*D10</f>
         <v>4.7310318434733993</v>
       </c>
-      <c r="F10" s="40"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="11">
         <v>7</v>
@@ -3423,48 +3385,43 @@
       </c>
       <c r="J10" s="11">
         <f t="shared" si="3"/>
-        <v>8.8785322958123274</v>
+        <v>8.2632237951821512</v>
       </c>
       <c r="K10" s="11">
         <f t="shared" si="4"/>
-        <v>0.99363685839462812</v>
-      </c>
-      <c r="L10" s="54">
+        <v>0.99265029543752825</v>
+      </c>
+      <c r="L10" s="48">
         <f t="shared" si="5"/>
-        <v>3.45650431426421</v>
-      </c>
-      <c r="M10" s="55"/>
+        <v>3.1869997468227331</v>
+      </c>
+      <c r="M10" s="49"/>
       <c r="N10" s="11">
         <f t="shared" si="7"/>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O10" s="11">
         <f t="shared" si="0"/>
-        <v>4.0259216999749121</v>
+        <v>3.7114997046265219</v>
       </c>
       <c r="P10" s="11">
         <f t="shared" si="1"/>
-        <v>4.5369206460749121</v>
+        <v>4.2224986507265214</v>
       </c>
       <c r="Q10" s="11">
         <f>9.10938356*10^(-31)*J10*299792458*K10/(1.60217662*10^(-19)*D15)</f>
-        <v>6.0009984271746371E-2</v>
+        <v>5.579566169143494E-2</v>
       </c>
       <c r="R10" s="11">
         <f t="shared" si="6"/>
-        <v>600.09984271746373</v>
-      </c>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="22"/>
+        <v>557.95661691434941</v>
+      </c>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="21"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -3473,7 +3430,7 @@
       <c r="D11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="42" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -3489,44 +3446,39 @@
       </c>
       <c r="J11" s="11">
         <f t="shared" si="3"/>
-        <v>9.9928543312226896</v>
+        <v>9.2896446162167763</v>
       </c>
       <c r="K11" s="11">
         <f t="shared" si="4"/>
-        <v>0.99498024770829652</v>
-      </c>
-      <c r="L11" s="54">
+        <v>0.99418920654475318</v>
+      </c>
+      <c r="L11" s="48">
         <f t="shared" si="5"/>
-        <v>4.0259216999749121</v>
-      </c>
-      <c r="M11" s="55"/>
+        <v>3.7114997046265219</v>
+      </c>
+      <c r="M11" s="49"/>
       <c r="N11" s="11">
         <f t="shared" si="7"/>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O11" s="11">
         <f t="shared" si="0"/>
-        <v>4.5953390856856142</v>
+        <v>4.2359996624303111</v>
       </c>
       <c r="P11" s="11">
         <f t="shared" si="1"/>
-        <v>5.1063380317856142</v>
+        <v>4.7469986085303111</v>
       </c>
       <c r="Q11" s="11">
         <f>9.10938356*10^(-31)*J11*299792458*K11/(1.60217662*10^(-19)*D15)</f>
-        <v>6.7633000795138704E-2</v>
+        <v>6.2823595039365798E-2</v>
       </c>
       <c r="R11" s="11">
         <f t="shared" si="6"/>
-        <v>676.33000795138707</v>
-      </c>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="22"/>
+        <v>628.23595039365796</v>
+      </c>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="21"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
@@ -3544,7 +3496,7 @@
       <c r="E12" s="8">
         <v>0.5</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="43">
         <v>0.26179938779914941</v>
       </c>
       <c r="G12" s="17"/>
@@ -3557,52 +3509,47 @@
       </c>
       <c r="J12" s="11">
         <f t="shared" si="3"/>
-        <v>11.107176366633052</v>
+        <v>10.316065437251398</v>
       </c>
       <c r="K12" s="11">
         <f t="shared" si="4"/>
-        <v>0.99593888371412997</v>
-      </c>
-      <c r="L12" s="54">
+        <v>0.99529059905043404</v>
+      </c>
+      <c r="L12" s="48">
         <f t="shared" si="5"/>
-        <v>4.5953390856856142</v>
-      </c>
-      <c r="M12" s="55"/>
+        <v>4.2359996624303111</v>
+      </c>
+      <c r="M12" s="49"/>
       <c r="N12" s="11">
         <f t="shared" si="7"/>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O12" s="11">
         <f t="shared" si="0"/>
-        <v>5.1647564713963163</v>
+        <v>4.7604996202340999</v>
       </c>
       <c r="P12" s="11">
         <f t="shared" si="1"/>
-        <v>5.6757554174963163</v>
+        <v>5.2714985663340999</v>
       </c>
       <c r="Q12" s="11">
         <f>9.10938356*10^(-31)*J12*299792458*K12/(1.60217662*10^(-19)*D15)</f>
-        <v>7.5247313212050498E-2</v>
+        <v>6.9842315854440298E-2</v>
       </c>
       <c r="R12" s="11">
         <f t="shared" si="6"/>
-        <v>752.47313212050494</v>
-      </c>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="22"/>
+        <v>698.42315854440301</v>
+      </c>
+      <c r="X12" s="31"/>
+      <c r="Y12" s="21"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="39"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="38"/>
       <c r="G13" s="17"/>
       <c r="H13" s="11">
         <v>10</v>
@@ -3613,44 +3560,39 @@
       </c>
       <c r="J13" s="11">
         <f t="shared" si="3"/>
-        <v>12.221498402043414</v>
+        <v>11.342486258286021</v>
       </c>
       <c r="K13" s="11">
         <f t="shared" si="4"/>
-        <v>0.99664687435852295</v>
-      </c>
-      <c r="L13" s="54">
+        <v>0.99610596470087587</v>
+      </c>
+      <c r="L13" s="48">
         <f t="shared" si="5"/>
-        <v>5.1647564713963163</v>
-      </c>
-      <c r="M13" s="55"/>
+        <v>4.7604996202340999</v>
+      </c>
+      <c r="M13" s="49"/>
       <c r="N13" s="11">
         <f t="shared" si="7"/>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="O13" s="11">
         <f t="shared" si="0"/>
-        <v>5.7341738571070184</v>
+        <v>5.2849995780378887</v>
       </c>
       <c r="P13" s="11">
         <f t="shared" si="1"/>
-        <v>6.2451728032070184</v>
+        <v>5.7959985241378886</v>
       </c>
       <c r="Q13" s="11">
         <f>9.10938356*10^(-31)*J13*299792458*K13/(1.60217662*10^(-19)*D15)</f>
-        <v>8.2855321250519753E-2</v>
+        <v>7.6854348180884269E-2</v>
       </c>
       <c r="R13" s="11">
         <f t="shared" si="6"/>
-        <v>828.55321250519751</v>
-      </c>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="22"/>
+        <v>768.54348180884267</v>
+      </c>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="21"/>
     </row>
     <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
@@ -3681,15 +3623,8 @@
       <c r="N14" s="57"/>
       <c r="O14" s="57"/>
       <c r="P14" s="57"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="22"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="21"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
@@ -3708,7 +3643,7 @@
         <f>E10/(B15+1)</f>
         <v>0.78850530724556656</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="39">
         <f>PI()/(2*C15)</f>
         <v>0.26179938779914941</v>
       </c>
@@ -3716,64 +3651,50 @@
       <c r="H15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="52" t="s">
+      <c r="I15" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
       <c r="L15" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="M15" s="53" t="s">
+      <c r="M15" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="N15" s="62"/>
-      <c r="O15" s="62"/>
-      <c r="P15" s="62"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="32"/>
-      <c r="Y15" s="22"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="X15" s="31"/>
+      <c r="Y15" s="21"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="38"/>
       <c r="G16" s="17"/>
       <c r="H16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="61" t="s">
+      <c r="I16" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
       <c r="L16" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="M16" s="62" t="s">
+      <c r="M16" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="N16" s="62"/>
-      <c r="O16" s="62"/>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="32"/>
-      <c r="Y16" s="22"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="44"/>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="21"/>
     </row>
     <row r="17" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
@@ -3796,29 +3717,22 @@
       <c r="H17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="61" t="s">
+      <c r="I17" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
       <c r="L17" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="M17" s="62" t="s">
+      <c r="M17" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="N17" s="62"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="22"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="21"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
@@ -3827,82 +3741,68 @@
       </c>
       <c r="C18" s="1">
         <f>SQRT(C21)*SQRT(C7*0.001)*COS(F12)</f>
-        <v>0.56941738571070166</v>
+        <v>0.52449995780378889</v>
       </c>
       <c r="D18" s="1">
         <f>C18*C15</f>
-        <v>3.41650431426421</v>
+        <v>3.1469997468227335</v>
       </c>
       <c r="E18" s="1">
         <f>B18+D18</f>
-        <v>3.45650431426421</v>
+        <v>3.1869997468227336</v>
       </c>
       <c r="F18" s="1">
         <f>D21/(1000*(C10-B10))</f>
-        <v>1.0438778412349299</v>
+        <v>0.96153348566389041</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="61" t="s">
+      <c r="I18" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="62"/>
-      <c r="K18" s="62"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
       <c r="L18" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="M18" s="53" t="s">
+      <c r="M18" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="N18" s="62"/>
-      <c r="O18" s="62"/>
-      <c r="P18" s="62"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="32"/>
-      <c r="Y18" s="22"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="21"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="38"/>
       <c r="G19" s="17"/>
       <c r="H19" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="61" t="s">
+      <c r="I19" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="J19" s="62"/>
-      <c r="K19" s="62"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
       <c r="L19" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="M19" s="62" t="s">
+      <c r="M19" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="N19" s="62"/>
-      <c r="O19" s="62"/>
-      <c r="P19" s="62"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="32"/>
-      <c r="Y19" s="22"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="44"/>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="21"/>
     </row>
     <row r="20" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
@@ -3918,30 +3818,25 @@
       <c r="E20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="40"/>
+      <c r="F20" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="G20" s="17"/>
       <c r="H20" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="51"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="55"/>
       <c r="L20" s="15"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="32"/>
-      <c r="Y20" s="22"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="44"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="21"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
@@ -3955,66 +3850,55 @@
       </c>
       <c r="D21" s="1">
         <f>SQRT(C7*C21*1000)</f>
-        <v>589.50425613767027</v>
+        <v>543.00231294035632</v>
       </c>
       <c r="E21" s="1">
-        <v>6</v>
-      </c>
-      <c r="F21" s="40"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <f>D21/(1000*LN(C10/B10)*B10)</f>
+        <v>2.0807993871239607</v>
+      </c>
       <c r="G21" s="17"/>
       <c r="H21" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="52" t="s">
+      <c r="I21" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
       <c r="L21" s="15"/>
-      <c r="M21" s="62"/>
-      <c r="N21" s="62"/>
-      <c r="O21" s="62"/>
-      <c r="P21" s="62"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="32"/>
-      <c r="Y21" s="22"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="X21" s="31"/>
+      <c r="Y21" s="21"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="39"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="38"/>
       <c r="G22" s="17"/>
       <c r="H22" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="52" t="s">
+      <c r="I22" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
       <c r="L22" s="15"/>
-      <c r="M22" s="62"/>
-      <c r="N22" s="62"/>
-      <c r="O22" s="62"/>
-      <c r="P22" s="62"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="32"/>
-      <c r="Y22" s="22"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="44"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="21"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
@@ -4037,25 +3921,18 @@
       <c r="H23" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="52" t="s">
+      <c r="I23" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
       <c r="L23" s="15"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="21"/>
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="32"/>
-      <c r="Y23" s="22"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44"/>
+      <c r="X23" s="31"/>
+      <c r="Y23" s="21"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
@@ -4075,62 +3952,48 @@
       </c>
       <c r="F24" s="1">
         <f>D21/(1000*(C10-B10-F27))</f>
-        <v>1.0626957640664163</v>
+        <v>0.97886699176811776</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="52" t="s">
+      <c r="I24" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
       <c r="L24" s="15"/>
-      <c r="M24" s="62"/>
-      <c r="N24" s="62"/>
-      <c r="O24" s="62"/>
-      <c r="P24" s="62"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="21"/>
-      <c r="S24" s="21"/>
-      <c r="T24" s="21"/>
-      <c r="U24" s="21"/>
-      <c r="V24" s="21"/>
-      <c r="W24" s="21"/>
-      <c r="X24" s="32"/>
-      <c r="Y24" s="22"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="21"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="39"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="17"/>
       <c r="H25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I25" s="61" t="s">
+      <c r="I25" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
       <c r="L25" s="15"/>
-      <c r="M25" s="62"/>
-      <c r="N25" s="62"/>
-      <c r="O25" s="62"/>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="21"/>
-      <c r="S25" s="21"/>
-      <c r="T25" s="21"/>
-      <c r="U25" s="21"/>
-      <c r="V25" s="21"/>
-      <c r="W25" s="21"/>
-      <c r="X25" s="32"/>
-      <c r="Y25" s="22"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
+      <c r="X25" s="31"/>
+      <c r="Y25" s="21"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
@@ -4140,8 +4003,8 @@
       <c r="C26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="6" t="s">
         <v>90</v>
       </c>
@@ -4149,38 +4012,34 @@
       <c r="H26" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I26" s="61" t="s">
+      <c r="I26" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
       <c r="L26" s="15"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="62"/>
-      <c r="O26" s="62"/>
-      <c r="P26" s="62"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-      <c r="T26" s="21"/>
-      <c r="U26" s="21"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="21"/>
-      <c r="X26" s="32"/>
-      <c r="Y26" s="22"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="21"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="1">
         <f>(E18/B24)+1</f>
-        <v>7.7642102604019643</v>
+        <v>7.2368029741475306</v>
       </c>
       <c r="C27" s="1">
         <f>SQRT(1-1/(B27*B27))</f>
-        <v>0.99167109701853262</v>
-      </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
+        <v>0.99040677432531854</v>
+      </c>
+      <c r="D27" s="22">
+        <f>2.14*(D4)^(1/4)*(C7*1000)^(1/2)</f>
+        <v>524.70848043442925</v>
+      </c>
+      <c r="E27" s="22"/>
       <c r="F27" s="1">
         <v>0.01</v>
       </c>
@@ -4188,103 +4047,108 @@
       <c r="H27" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I27" s="61" t="s">
+      <c r="I27" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
       <c r="L27" s="15"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="62"/>
-      <c r="O27" s="62"/>
-      <c r="P27" s="62"/>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="21"/>
-      <c r="S27" s="21"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="21"/>
-      <c r="V27" s="21"/>
-      <c r="W27" s="21"/>
-      <c r="X27" s="32"/>
-      <c r="Y27" s="22"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="X27" s="31"/>
+      <c r="Y27" s="21"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="41" t="s">
+      <c r="A28" s="24"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="G28" s="26"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I28" s="53" t="s">
+      <c r="I28" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
       <c r="L28" s="15"/>
-      <c r="M28" s="62"/>
-      <c r="N28" s="62"/>
-      <c r="O28" s="62"/>
-      <c r="P28" s="62"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="37"/>
-      <c r="S28" s="37"/>
-      <c r="T28" s="37"/>
-      <c r="U28" s="37"/>
-      <c r="V28" s="37"/>
-      <c r="W28" s="37"/>
-      <c r="X28" s="38"/>
-      <c r="Y28" s="22"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="44"/>
+      <c r="Q28" s="36"/>
+      <c r="R28" s="36"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="36"/>
+      <c r="U28" s="36"/>
+      <c r="V28" s="36"/>
+      <c r="W28" s="36"/>
+      <c r="X28" s="37"/>
+      <c r="Y28" s="21"/>
     </row>
     <row r="29" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
-      <c r="P29" s="28"/>
-      <c r="Q29" s="28"/>
-      <c r="R29" s="28"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="28"/>
-      <c r="U29" s="28"/>
-      <c r="V29" s="28"/>
-      <c r="W29" s="28"/>
-      <c r="X29" s="28"/>
-      <c r="Y29" s="29"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27"/>
+      <c r="V29" s="27"/>
+      <c r="W29" s="27"/>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="H14:P14"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="H2:R2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
     <mergeCell ref="M28:P28"/>
     <mergeCell ref="I26:K26"/>
     <mergeCell ref="I27:K27"/>
@@ -4301,33 +4165,6 @@
     <mergeCell ref="M24:P24"/>
     <mergeCell ref="M25:P25"/>
     <mergeCell ref="M26:P26"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="H14:P14"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="H2:R2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
   </mergeCells>
   <conditionalFormatting sqref="K4:K13">
     <cfRule type="colorScale" priority="4">

</xml_diff>

<commit_message>
multhtreading added GUI started
</commit_message>
<xml_diff>
--- a/documents/Rhodotron Parametreler (v5).xlsx
+++ b/documents/Rhodotron Parametreler (v5).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Repos\MSThesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AE587A-32BB-4D47-8742-3DA4E9AA6100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC56105-A168-4F4C-AC26-0C0FD646D489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A977ED4B-B779-4DB6-A8B8-B7CE20AE608B}"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="28800" windowHeight="15345" xr2:uid="{A977ED4B-B779-4DB6-A8B8-B7CE20AE608B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -2337,56 +2337,56 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2881,8 +2881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65439ADF-7CD5-4C3B-BCA2-78038D935A1F}">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2907,42 +2907,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="52"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="46"/>
     </row>
     <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="60"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
@@ -3045,36 +3045,36 @@
       </c>
       <c r="J4" s="11">
         <f>P4/0.5109989461</f>
-        <v>2.1046988689744164</v>
+        <v>1.6192493199880396</v>
       </c>
       <c r="K4" s="11">
         <f>SQRT(1-(1/(J4*J4)))</f>
-        <v>0.87991704128853487</v>
-      </c>
-      <c r="L4" s="48">
+        <v>0.78651582595913017</v>
+      </c>
+      <c r="L4" s="52">
         <f>B18</f>
         <v>0.04</v>
       </c>
-      <c r="M4" s="49"/>
+      <c r="M4" s="53"/>
       <c r="N4" s="11">
         <f>C18</f>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O4" s="11">
         <f t="shared" ref="O4:O13" si="0">L4+N4</f>
-        <v>0.56449995780378892</v>
+        <v>0.31643574988702983</v>
       </c>
       <c r="P4" s="12">
         <f t="shared" ref="P4:P13" si="1">O4+0.5109989461</f>
-        <v>1.0754989039037888</v>
+        <v>0.82743469598702979</v>
       </c>
       <c r="Q4" s="12">
         <f>9.10938356*10^(-31)*J4*299792458*K4/(1.60217662*10^(-19)*D15)</f>
-        <v>1.2597557158046826E-2</v>
+        <v>8.6631499213536724E-3</v>
       </c>
       <c r="R4" s="12">
         <f>Q4*10000</f>
-        <v>125.97557158046826</v>
+        <v>86.631499213536728</v>
       </c>
       <c r="X4" s="31"/>
       <c r="Y4" s="21"/>
@@ -3096,36 +3096,36 @@
       </c>
       <c r="J5" s="11">
         <f t="shared" ref="J5:J13" si="3">P5/0.5109989461</f>
-        <v>3.1311196900090397</v>
+        <v>2.1602205920362851</v>
       </c>
       <c r="K5" s="11">
         <f t="shared" ref="K5:K13" si="4">SQRT(1-(1/(J5*J5)))</f>
-        <v>0.94762855854960959</v>
-      </c>
-      <c r="L5" s="48">
+        <v>0.88640231638164779</v>
+      </c>
+      <c r="L5" s="52">
         <f t="shared" ref="L5:L13" si="5">O4</f>
-        <v>0.56449995780378892</v>
-      </c>
-      <c r="M5" s="49"/>
+        <v>0.31643574988702983</v>
+      </c>
+      <c r="M5" s="53"/>
       <c r="N5" s="11">
         <f>N4</f>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O5" s="11">
         <f t="shared" si="0"/>
-        <v>1.0889999156075778</v>
+        <v>0.59287149977405962</v>
       </c>
       <c r="P5" s="11">
         <f t="shared" si="1"/>
-        <v>1.5999988617075778</v>
+        <v>1.1038704458740596</v>
       </c>
       <c r="Q5" s="11">
         <f>9.10938356*10^(-31)*J5*299792458*K5/(1.60217662*10^(-19)*D15)</f>
-        <v>2.0183312797937007E-2</v>
+        <v>1.3025176741189123E-2</v>
       </c>
       <c r="R5" s="11">
         <f t="shared" ref="R5:R13" si="6">Q5*10000</f>
-        <v>201.83312797937006</v>
+        <v>130.25176741189122</v>
       </c>
       <c r="X5" s="31"/>
       <c r="Y5" s="21"/>
@@ -3153,36 +3153,36 @@
       </c>
       <c r="J6" s="11">
         <f t="shared" si="3"/>
-        <v>4.1575405110436625</v>
+        <v>2.7011918640845303</v>
       </c>
       <c r="K6" s="11">
         <f t="shared" si="4"/>
-        <v>0.97064249270561198</v>
-      </c>
-      <c r="L6" s="48">
+        <v>0.9289493067689707</v>
+      </c>
+      <c r="L6" s="52">
         <f t="shared" si="5"/>
-        <v>1.0889999156075778</v>
-      </c>
-      <c r="M6" s="49"/>
+        <v>0.59287149977405962</v>
+      </c>
+      <c r="M6" s="53"/>
       <c r="N6" s="11">
         <f t="shared" ref="N6:N13" si="7">N5</f>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O6" s="11">
         <f t="shared" si="0"/>
-        <v>1.6134998734113668</v>
+        <v>0.86930724966108941</v>
       </c>
       <c r="P6" s="11">
         <f t="shared" si="1"/>
-        <v>2.1244988195113668</v>
+        <v>1.3803061957610894</v>
       </c>
       <c r="Q6" s="11">
         <f>9.10938356*10^(-31)*J6*299792458*K6/(1.60217662*10^(-19)*D15)</f>
-        <v>2.7450510829572693E-2</v>
+        <v>1.7068764603662655E-2</v>
       </c>
       <c r="R6" s="11">
         <f t="shared" si="6"/>
-        <v>274.50510829572693</v>
+        <v>170.68764603662655</v>
       </c>
       <c r="X6" s="31"/>
       <c r="Y6" s="21"/>
@@ -3191,14 +3191,14 @@
       <c r="A7" s="16"/>
       <c r="B7" s="1">
         <f>C7+D7</f>
-        <v>39.186999746822735</v>
+        <v>11.698614499322179</v>
       </c>
       <c r="C7" s="1">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <f>E18*E21</f>
-        <v>3.1869997468227336</v>
+        <v>1.6986144993221792</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="39"/>
@@ -3212,36 +3212,36 @@
       </c>
       <c r="J7" s="11">
         <f t="shared" si="3"/>
-        <v>5.1839613320782849</v>
+        <v>3.2421631361327758</v>
       </c>
       <c r="K7" s="11">
         <f t="shared" si="4"/>
-        <v>0.98121789556513939</v>
-      </c>
-      <c r="L7" s="48">
+        <v>0.95124507955588811</v>
+      </c>
+      <c r="L7" s="52">
         <f t="shared" si="5"/>
-        <v>1.6134998734113668</v>
-      </c>
-      <c r="M7" s="49"/>
+        <v>0.86930724966108941</v>
+      </c>
+      <c r="M7" s="53"/>
       <c r="N7" s="11">
         <f t="shared" si="7"/>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O7" s="11">
         <f t="shared" si="0"/>
-        <v>2.1379998312151556</v>
+        <v>1.1457429995481192</v>
       </c>
       <c r="P7" s="11">
         <f t="shared" si="1"/>
-        <v>2.6489987773151555</v>
+        <v>1.6567419456481192</v>
       </c>
       <c r="Q7" s="11">
         <f>9.10938356*10^(-31)*J7*299792458*K7/(1.60217662*10^(-19)*D15)</f>
-        <v>3.4600458584614406E-2</v>
+        <v>2.0978862086108233E-2</v>
       </c>
       <c r="R7" s="11">
         <f t="shared" si="6"/>
-        <v>346.00458584614404</v>
+        <v>209.78862086108234</v>
       </c>
       <c r="X7" s="31"/>
       <c r="Y7" s="21"/>
@@ -3263,36 +3263,36 @@
       </c>
       <c r="J8" s="11">
         <f t="shared" si="3"/>
-        <v>6.2103821531129073</v>
+        <v>3.7831344081810214</v>
       </c>
       <c r="K8" s="11">
         <f t="shared" si="4"/>
-        <v>0.98695103140982687</v>
-      </c>
-      <c r="L8" s="48">
+        <v>0.96443199899784426</v>
+      </c>
+      <c r="L8" s="52">
         <f t="shared" si="5"/>
-        <v>2.1379998312151556</v>
-      </c>
-      <c r="M8" s="49"/>
+        <v>1.1457429995481192</v>
+      </c>
+      <c r="M8" s="53"/>
       <c r="N8" s="11">
         <f t="shared" si="7"/>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O8" s="11">
         <f t="shared" si="0"/>
-        <v>2.6624997890189444</v>
+        <v>1.422178749435149</v>
       </c>
       <c r="P8" s="11">
         <f t="shared" si="1"/>
-        <v>3.1734987351189443</v>
+        <v>1.933177695535149</v>
       </c>
       <c r="Q8" s="11">
         <f>9.10938356*10^(-31)*J8*299792458*K8/(1.60217662*10^(-19)*D15)</f>
-        <v>4.1693520886137168E-2</v>
+        <v>2.481864253212333E-2</v>
       </c>
       <c r="R8" s="11">
         <f t="shared" si="6"/>
-        <v>416.93520886137168</v>
+        <v>248.18642532123329</v>
       </c>
       <c r="X8" s="31"/>
       <c r="Y8" s="21"/>
@@ -3322,36 +3322,36 @@
       </c>
       <c r="J9" s="11">
         <f t="shared" si="3"/>
-        <v>7.2368029741475297</v>
+        <v>4.324105680229267</v>
       </c>
       <c r="K9" s="11">
         <f t="shared" si="4"/>
-        <v>0.99040677432531854</v>
-      </c>
-      <c r="L9" s="48">
+        <v>0.97289158151619393</v>
+      </c>
+      <c r="L9" s="52">
         <f t="shared" si="5"/>
-        <v>2.6624997890189444</v>
-      </c>
-      <c r="M9" s="49"/>
+        <v>1.422178749435149</v>
+      </c>
+      <c r="M9" s="53"/>
       <c r="N9" s="11">
         <f t="shared" si="7"/>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O9" s="11">
         <f t="shared" si="0"/>
-        <v>3.1869997468227331</v>
+        <v>1.6986144993221788</v>
       </c>
       <c r="P9" s="11">
         <f t="shared" si="1"/>
-        <v>3.6979986929227331</v>
+        <v>2.2096134454221787</v>
       </c>
       <c r="Q9" s="11">
         <f>9.10938356*10^(-31)*J9*299792458*K9/(1.60217662*10^(-19)*D15)</f>
-        <v>4.8754532031965031E-2</v>
+        <v>2.8616425584327653E-2</v>
       </c>
       <c r="R9" s="11">
         <f t="shared" si="6"/>
-        <v>487.54532031965033</v>
+        <v>286.16425584327652</v>
       </c>
       <c r="X9" s="31"/>
       <c r="Y9" s="21"/>
@@ -3385,36 +3385,36 @@
       </c>
       <c r="J10" s="11">
         <f t="shared" si="3"/>
-        <v>8.2632237951821512</v>
+        <v>4.8650769522775121</v>
       </c>
       <c r="K10" s="11">
         <f t="shared" si="4"/>
-        <v>0.99265029543752825</v>
-      </c>
-      <c r="L10" s="48">
+        <v>0.97864733047660457</v>
+      </c>
+      <c r="L10" s="52">
         <f t="shared" si="5"/>
-        <v>3.1869997468227331</v>
-      </c>
-      <c r="M10" s="49"/>
+        <v>1.6986144993221788</v>
+      </c>
+      <c r="M10" s="53"/>
       <c r="N10" s="11">
         <f t="shared" si="7"/>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O10" s="11">
         <f t="shared" si="0"/>
-        <v>3.7114997046265219</v>
+        <v>1.9750502492092086</v>
       </c>
       <c r="P10" s="11">
         <f t="shared" si="1"/>
-        <v>4.2224986507265214</v>
+        <v>2.4860491953092083</v>
       </c>
       <c r="Q10" s="11">
         <f>9.10938356*10^(-31)*J10*299792458*K10/(1.60217662*10^(-19)*D15)</f>
-        <v>5.579566169143494E-2</v>
+        <v>3.2386988786950725E-2</v>
       </c>
       <c r="R10" s="11">
         <f t="shared" si="6"/>
-        <v>557.95661691434941</v>
+        <v>323.86988786950724</v>
       </c>
       <c r="X10" s="31"/>
       <c r="Y10" s="21"/>
@@ -3446,36 +3446,36 @@
       </c>
       <c r="J11" s="11">
         <f t="shared" si="3"/>
-        <v>9.2896446162167763</v>
+        <v>5.4060482243257573</v>
       </c>
       <c r="K11" s="11">
         <f t="shared" si="4"/>
-        <v>0.99418920654475318</v>
-      </c>
-      <c r="L11" s="48">
+        <v>0.98274266149631473</v>
+      </c>
+      <c r="L11" s="52">
         <f t="shared" si="5"/>
-        <v>3.7114997046265219</v>
-      </c>
-      <c r="M11" s="49"/>
+        <v>1.9750502492092086</v>
+      </c>
+      <c r="M11" s="53"/>
       <c r="N11" s="11">
         <f t="shared" si="7"/>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O11" s="11">
         <f t="shared" si="0"/>
-        <v>4.2359996624303111</v>
+        <v>2.2514859990962384</v>
       </c>
       <c r="P11" s="11">
         <f t="shared" si="1"/>
-        <v>4.7469986085303111</v>
+        <v>2.7624849451962383</v>
       </c>
       <c r="Q11" s="11">
         <f>9.10938356*10^(-31)*J11*299792458*K11/(1.60217662*10^(-19)*D15)</f>
-        <v>6.2823595039365798E-2</v>
+        <v>3.6138853129636689E-2</v>
       </c>
       <c r="R11" s="11">
         <f t="shared" si="6"/>
-        <v>628.23595039365796</v>
+        <v>361.38853129636686</v>
       </c>
       <c r="X11" s="31"/>
       <c r="Y11" s="21"/>
@@ -3509,36 +3509,36 @@
       </c>
       <c r="J12" s="11">
         <f t="shared" si="3"/>
-        <v>10.316065437251398</v>
+        <v>5.9470194963740033</v>
       </c>
       <c r="K12" s="11">
         <f t="shared" si="4"/>
-        <v>0.99529059905043404</v>
-      </c>
-      <c r="L12" s="48">
+        <v>0.98576117144056086</v>
+      </c>
+      <c r="L12" s="52">
         <f t="shared" si="5"/>
-        <v>4.2359996624303111</v>
-      </c>
-      <c r="M12" s="49"/>
+        <v>2.2514859990962384</v>
+      </c>
+      <c r="M12" s="53"/>
       <c r="N12" s="11">
         <f t="shared" si="7"/>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O12" s="11">
         <f t="shared" si="0"/>
-        <v>4.7604996202340999</v>
+        <v>2.5279217489832684</v>
       </c>
       <c r="P12" s="11">
         <f t="shared" si="1"/>
-        <v>5.2714985663340999</v>
+        <v>3.0389206950832683</v>
       </c>
       <c r="Q12" s="11">
         <f>9.10938356*10^(-31)*J12*299792458*K12/(1.60217662*10^(-19)*D15)</f>
-        <v>6.9842315854440298E-2</v>
+        <v>3.9877296820891715E-2</v>
       </c>
       <c r="R12" s="11">
         <f t="shared" si="6"/>
-        <v>698.42315854440301</v>
+        <v>398.77296820891718</v>
       </c>
       <c r="X12" s="31"/>
       <c r="Y12" s="21"/>
@@ -3560,36 +3560,36 @@
       </c>
       <c r="J13" s="11">
         <f t="shared" si="3"/>
-        <v>11.342486258286021</v>
+        <v>6.4879907684222493</v>
       </c>
       <c r="K13" s="11">
         <f t="shared" si="4"/>
-        <v>0.99610596470087587</v>
-      </c>
-      <c r="L13" s="48">
+        <v>0.98805043334790232</v>
+      </c>
+      <c r="L13" s="52">
         <f t="shared" si="5"/>
-        <v>4.7604996202340999</v>
-      </c>
-      <c r="M13" s="49"/>
+        <v>2.5279217489832684</v>
+      </c>
+      <c r="M13" s="53"/>
       <c r="N13" s="11">
         <f t="shared" si="7"/>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="O13" s="11">
         <f t="shared" si="0"/>
-        <v>5.2849995780378887</v>
+        <v>2.8043574988702984</v>
       </c>
       <c r="P13" s="11">
         <f t="shared" si="1"/>
-        <v>5.7959985241378886</v>
+        <v>3.3153564449702984</v>
       </c>
       <c r="Q13" s="11">
         <f>9.10938356*10^(-31)*J13*299792458*K13/(1.60217662*10^(-19)*D15)</f>
-        <v>7.6854348180884269E-2</v>
+        <v>4.3605771766295091E-2</v>
       </c>
       <c r="R13" s="11">
         <f t="shared" si="6"/>
-        <v>768.54348180884267</v>
+        <v>436.05771766295089</v>
       </c>
       <c r="X13" s="31"/>
       <c r="Y13" s="21"/>
@@ -3612,17 +3612,17 @@
         <v>73</v>
       </c>
       <c r="G14" s="17"/>
-      <c r="H14" s="56" t="s">
+      <c r="H14" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="55"/>
+      <c r="P14" s="55"/>
       <c r="X14" s="31"/>
       <c r="Y14" s="21"/>
     </row>
@@ -3651,20 +3651,20 @@
       <c r="H15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="47" t="s">
+      <c r="I15" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
       <c r="L15" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="M15" s="46" t="s">
+      <c r="M15" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
       <c r="X15" s="31"/>
       <c r="Y15" s="21"/>
     </row>
@@ -3679,20 +3679,20 @@
       <c r="H16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="45" t="s">
+      <c r="I16" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
       <c r="L16" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="M16" s="44" t="s">
+      <c r="M16" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
       <c r="X16" s="31"/>
       <c r="Y16" s="21"/>
     </row>
@@ -3717,20 +3717,20 @@
       <c r="H17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="45" t="s">
+      <c r="I17" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
       <c r="L17" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="M17" s="44" t="s">
+      <c r="M17" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="N17" s="44"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
       <c r="X17" s="31"/>
       <c r="Y17" s="21"/>
     </row>
@@ -3741,38 +3741,38 @@
       </c>
       <c r="C18" s="1">
         <f>SQRT(C21)*SQRT(C7*0.001)*COS(F12)</f>
-        <v>0.52449995780378889</v>
+        <v>0.27643574988702985</v>
       </c>
       <c r="D18" s="1">
         <f>C18*C15</f>
-        <v>3.1469997468227335</v>
+        <v>1.6586144993221792</v>
       </c>
       <c r="E18" s="1">
         <f>B18+D18</f>
-        <v>3.1869997468227336</v>
+        <v>1.6986144993221792</v>
       </c>
       <c r="F18" s="1">
         <f>D21/(1000*(C10-B10))</f>
-        <v>0.96153348566389041</v>
+        <v>0.50677264353645879</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="45" t="s">
+      <c r="I18" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
       <c r="L18" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="M18" s="46" t="s">
+      <c r="M18" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="N18" s="44"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="44"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
       <c r="X18" s="31"/>
       <c r="Y18" s="21"/>
     </row>
@@ -3787,20 +3787,20 @@
       <c r="H19" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="45" t="s">
+      <c r="I19" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
       <c r="L19" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="M19" s="44" t="s">
+      <c r="M19" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
       <c r="X19" s="31"/>
       <c r="Y19" s="21"/>
     </row>
@@ -3825,16 +3825,16 @@
       <c r="H20" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="53" t="s">
+      <c r="I20" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="J20" s="54"/>
-      <c r="K20" s="55"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="49"/>
       <c r="L20" s="15"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="44"/>
-      <c r="P20" s="44"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="60"/>
+      <c r="P20" s="60"/>
       <c r="X20" s="31"/>
       <c r="Y20" s="21"/>
     </row>
@@ -3850,29 +3850,29 @@
       </c>
       <c r="D21" s="1">
         <f>SQRT(C7*C21*1000)</f>
-        <v>543.00231294035632</v>
+        <v>286.1873472718413</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
       </c>
       <c r="F21" s="1">
         <f>D21/(1000*LN(C10/B10)*B10)</f>
-        <v>2.0807993871239607</v>
+        <v>1.0966775695323592</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="47" t="s">
+      <c r="I21" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
       <c r="L21" s="15"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="44"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
       <c r="X21" s="31"/>
       <c r="Y21" s="21"/>
     </row>
@@ -3887,16 +3887,16 @@
       <c r="H22" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="47" t="s">
+      <c r="I22" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
       <c r="L22" s="15"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="44"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
+      <c r="P22" s="60"/>
       <c r="X22" s="31"/>
       <c r="Y22" s="21"/>
     </row>
@@ -3921,16 +3921,16 @@
       <c r="H23" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="47" t="s">
+      <c r="I23" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
       <c r="L23" s="15"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="44"/>
-      <c r="P23" s="44"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
       <c r="X23" s="31"/>
       <c r="Y23" s="21"/>
     </row>
@@ -3952,22 +3952,22 @@
       </c>
       <c r="F24" s="1">
         <f>D21/(1000*(C10-B10-F27))</f>
-        <v>0.97886699176811776</v>
+        <v>0.51590820339075727</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="47" t="s">
+      <c r="I24" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
       <c r="L24" s="15"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="44"/>
-      <c r="P24" s="44"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="60"/>
+      <c r="P24" s="60"/>
       <c r="X24" s="31"/>
       <c r="Y24" s="21"/>
     </row>
@@ -3982,16 +3982,16 @@
       <c r="H25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I25" s="45" t="s">
+      <c r="I25" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
       <c r="L25" s="15"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="44"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="60"/>
       <c r="X25" s="31"/>
       <c r="Y25" s="21"/>
     </row>
@@ -4012,16 +4012,16 @@
       <c r="H26" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I26" s="45" t="s">
+      <c r="I26" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
       <c r="L26" s="15"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="60"/>
       <c r="X26" s="31"/>
       <c r="Y26" s="21"/>
     </row>
@@ -4029,15 +4029,15 @@
       <c r="A27" s="16"/>
       <c r="B27" s="1">
         <f>(E18/B24)+1</f>
-        <v>7.2368029741475306</v>
+        <v>4.3241056802292679</v>
       </c>
       <c r="C27" s="1">
         <f>SQRT(1-1/(B27*B27))</f>
-        <v>0.99040677432531854</v>
+        <v>0.97289158151619393</v>
       </c>
       <c r="D27" s="22">
         <f>2.14*(D4)^(1/4)*(C7*1000)^(1/2)</f>
-        <v>524.70848043442925</v>
+        <v>276.54565096311552</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="1">
@@ -4047,16 +4047,16 @@
       <c r="H27" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I27" s="45" t="s">
+      <c r="I27" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
       <c r="L27" s="15"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
-      <c r="P27" s="44"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
       <c r="X27" s="31"/>
       <c r="Y27" s="21"/>
     </row>
@@ -4073,16 +4073,16 @@
       <c r="H28" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I28" s="46" t="s">
+      <c r="I28" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
       <c r="L28" s="15"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="44"/>
-      <c r="P28" s="44"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
       <c r="Q28" s="36"/>
       <c r="R28" s="36"/>
       <c r="S28" s="36"/>
@@ -4122,6 +4122,33 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="I17:K17"/>
     <mergeCell ref="A1:Y1"/>
     <mergeCell ref="I20:K20"/>
     <mergeCell ref="I21:K21"/>
@@ -4138,33 +4165,6 @@
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="M26:P26"/>
   </mergeCells>
   <conditionalFormatting sqref="K4:K13">
     <cfRule type="colorScale" priority="4">

</xml_diff>